<commit_message>
Renames and macro-free workbooks
</commit_message>
<xml_diff>
--- a/CompLaagRayon/files/template-excel-rk-indoor-indiv.xlsx
+++ b/CompLaagRayon/files/template-excel-rk-indoor-indiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\RK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130FE121-DF37-4DC5-96E3-35E4F4661F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B780EE6-F58C-4247-8557-892383029683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="660" windowWidth="22440" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="22440" windowHeight="14040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="3" r:id="rId1"/>
@@ -1021,6 +1021,24 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1073,24 +1091,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1456,7 +1456,7 @@
   <sheetPr codeName="Blad5"/>
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1824,24 +1824,24 @@
     <row r="2" spans="1:25" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
-      <c r="C2" s="117" t="s">
+      <c r="C2" s="122" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="118"/>
-      <c r="N2" s="118"/>
-      <c r="O2" s="118"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="118"/>
-      <c r="R2" s="119"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
+      <c r="R2" s="124"/>
       <c r="S2" s="63"/>
       <c r="T2" s="63"/>
       <c r="U2" s="63"/>
@@ -1851,29 +1851,29 @@
       <c r="A3" s="51"/>
       <c r="B3" s="51"/>
       <c r="C3" s="57"/>
-      <c r="D3" s="116" t="s">
+      <c r="D3" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="116"/>
+      <c r="E3" s="121"/>
       <c r="F3" s="111"/>
-      <c r="G3" s="130" t="s">
+      <c r="G3" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="123" t="s">
+      <c r="H3" s="128" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="123"/>
-      <c r="J3" s="121" t="s">
+      <c r="I3" s="128"/>
+      <c r="J3" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="121"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
-      <c r="N3" s="121"/>
-      <c r="O3" s="121"/>
-      <c r="P3" s="121"/>
-      <c r="Q3" s="121"/>
-      <c r="R3" s="122"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
+      <c r="Q3" s="126"/>
+      <c r="R3" s="127"/>
       <c r="S3" s="61"/>
       <c r="T3" s="61"/>
       <c r="U3" s="61"/>
@@ -1886,13 +1886,13 @@
       <c r="D4" s="60"/>
       <c r="E4" s="60"/>
       <c r="F4" s="58"/>
-      <c r="G4" s="127"/>
+      <c r="G4" s="113"/>
       <c r="H4" s="58"/>
       <c r="I4" s="59"/>
-      <c r="J4" s="120" t="s">
+      <c r="J4" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="120"/>
+      <c r="K4" s="125"/>
       <c r="L4" s="61"/>
       <c r="M4" s="61"/>
       <c r="N4" s="61"/>
@@ -1906,10 +1906,10 @@
       <c r="V4" s="2"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5" s="114" t="s">
+      <c r="A5" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="115"/>
+      <c r="B5" s="120"/>
       <c r="C5" s="18"/>
       <c r="D5" s="5" t="s">
         <v>0</v>
@@ -1985,7 +1985,7 @@
       <c r="A7" s="16">
         <v>1</v>
       </c>
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="117" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="19"/>
@@ -1998,7 +1998,7 @@
       <c r="F7" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G7" s="128">
+      <c r="G7" s="114">
         <v>100</v>
       </c>
       <c r="H7" s="8"/>
@@ -2030,12 +2030,12 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
-      <c r="B8" s="131"/>
+      <c r="B8" s="117"/>
       <c r="C8" s="19"/>
       <c r="D8" s="10"/>
       <c r="E8" s="8"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="128"/>
+      <c r="G8" s="114"/>
       <c r="H8" s="8"/>
       <c r="I8" s="11"/>
       <c r="J8" s="8"/>
@@ -2063,12 +2063,12 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
-      <c r="B9" s="131"/>
+      <c r="B9" s="117"/>
       <c r="C9" s="19"/>
       <c r="D9" s="10"/>
       <c r="E9" s="8"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="128"/>
+      <c r="G9" s="114"/>
       <c r="H9" s="8"/>
       <c r="I9" s="11"/>
       <c r="J9" s="8"/>
@@ -2096,12 +2096,12 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
-      <c r="B10" s="131"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="19"/>
       <c r="D10" s="10"/>
       <c r="E10" s="8"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="128"/>
+      <c r="G10" s="114"/>
       <c r="H10" s="8"/>
       <c r="I10" s="11"/>
       <c r="J10" s="8"/>
@@ -2129,12 +2129,12 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
-      <c r="B11" s="131"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="19"/>
       <c r="D11" s="10"/>
       <c r="E11" s="8"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="128"/>
+      <c r="G11" s="114"/>
       <c r="H11" s="8"/>
       <c r="I11" s="11"/>
       <c r="J11" s="8"/>
@@ -2162,12 +2162,12 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
-      <c r="B12" s="131"/>
+      <c r="B12" s="117"/>
       <c r="C12" s="19"/>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="128"/>
+      <c r="G12" s="114"/>
       <c r="H12" s="8"/>
       <c r="I12" s="11"/>
       <c r="J12" s="8"/>
@@ -2195,12 +2195,12 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
-      <c r="B13" s="131"/>
+      <c r="B13" s="117"/>
       <c r="C13" s="19"/>
       <c r="D13" s="10"/>
       <c r="E13" s="8"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="128"/>
+      <c r="G13" s="114"/>
       <c r="H13" s="8"/>
       <c r="I13" s="11"/>
       <c r="J13" s="8"/>
@@ -2228,12 +2228,12 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
-      <c r="B14" s="131"/>
+      <c r="B14" s="117"/>
       <c r="C14" s="19"/>
       <c r="D14" s="10"/>
       <c r="E14" s="8"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="128"/>
+      <c r="G14" s="114"/>
       <c r="H14" s="8"/>
       <c r="I14" s="11"/>
       <c r="J14" s="8"/>
@@ -2261,12 +2261,12 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="16"/>
-      <c r="B15" s="131"/>
+      <c r="B15" s="117"/>
       <c r="C15" s="19"/>
       <c r="D15" s="10"/>
       <c r="E15" s="8"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="128"/>
+      <c r="G15" s="114"/>
       <c r="H15" s="8"/>
       <c r="I15" s="11"/>
       <c r="J15" s="8"/>
@@ -2294,12 +2294,12 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
-      <c r="B16" s="131"/>
+      <c r="B16" s="117"/>
       <c r="C16" s="19"/>
       <c r="D16" s="10"/>
       <c r="E16" s="8"/>
       <c r="F16" s="10"/>
-      <c r="G16" s="128"/>
+      <c r="G16" s="114"/>
       <c r="H16" s="8"/>
       <c r="I16" s="11"/>
       <c r="J16" s="8"/>
@@ -2327,12 +2327,12 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
-      <c r="B17" s="131"/>
+      <c r="B17" s="117"/>
       <c r="C17" s="19"/>
       <c r="D17" s="10"/>
       <c r="E17" s="8"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="128"/>
+      <c r="G17" s="114"/>
       <c r="H17" s="8"/>
       <c r="I17" s="11"/>
       <c r="J17" s="8"/>
@@ -2360,12 +2360,12 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
-      <c r="B18" s="131"/>
+      <c r="B18" s="117"/>
       <c r="C18" s="19"/>
       <c r="D18" s="10"/>
       <c r="E18" s="8"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="128"/>
+      <c r="G18" s="114"/>
       <c r="H18" s="8"/>
       <c r="I18" s="11"/>
       <c r="J18" s="8"/>
@@ -2393,12 +2393,12 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
-      <c r="B19" s="131"/>
+      <c r="B19" s="117"/>
       <c r="C19" s="19"/>
       <c r="D19" s="10"/>
       <c r="E19" s="8"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="128"/>
+      <c r="G19" s="114"/>
       <c r="H19" s="8"/>
       <c r="I19" s="11"/>
       <c r="J19" s="8"/>
@@ -2426,12 +2426,12 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>
-      <c r="B20" s="131"/>
+      <c r="B20" s="117"/>
       <c r="C20" s="19"/>
       <c r="D20" s="10"/>
       <c r="E20" s="8"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="128"/>
+      <c r="G20" s="114"/>
       <c r="H20" s="8"/>
       <c r="I20" s="11"/>
       <c r="J20" s="8"/>
@@ -2459,12 +2459,12 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
-      <c r="B21" s="131"/>
+      <c r="B21" s="117"/>
       <c r="C21" s="19"/>
       <c r="D21" s="10"/>
       <c r="E21" s="8"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="128"/>
+      <c r="G21" s="114"/>
       <c r="H21" s="8"/>
       <c r="I21" s="11"/>
       <c r="J21" s="8"/>
@@ -2492,12 +2492,12 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="16"/>
-      <c r="B22" s="131"/>
+      <c r="B22" s="117"/>
       <c r="C22" s="19"/>
       <c r="D22" s="10"/>
       <c r="E22" s="8"/>
       <c r="F22" s="10"/>
-      <c r="G22" s="128"/>
+      <c r="G22" s="114"/>
       <c r="H22" s="8"/>
       <c r="I22" s="11"/>
       <c r="J22" s="8"/>
@@ -2525,12 +2525,12 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="16"/>
-      <c r="B23" s="131"/>
+      <c r="B23" s="117"/>
       <c r="C23" s="19"/>
       <c r="D23" s="10"/>
       <c r="E23" s="8"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="128"/>
+      <c r="G23" s="114"/>
       <c r="H23" s="8"/>
       <c r="I23" s="11"/>
       <c r="J23" s="8"/>
@@ -2558,12 +2558,12 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="16"/>
-      <c r="B24" s="131"/>
+      <c r="B24" s="117"/>
       <c r="C24" s="19"/>
       <c r="D24" s="10"/>
       <c r="E24" s="8"/>
       <c r="F24" s="10"/>
-      <c r="G24" s="128"/>
+      <c r="G24" s="114"/>
       <c r="H24" s="8"/>
       <c r="I24" s="11"/>
       <c r="J24" s="8"/>
@@ -2591,12 +2591,12 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="16"/>
-      <c r="B25" s="131"/>
+      <c r="B25" s="117"/>
       <c r="C25" s="19"/>
       <c r="D25" s="10"/>
       <c r="E25" s="8"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="128"/>
+      <c r="G25" s="114"/>
       <c r="H25" s="8"/>
       <c r="I25" s="11"/>
       <c r="J25" s="8"/>
@@ -2624,12 +2624,12 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="16"/>
-      <c r="B26" s="131"/>
+      <c r="B26" s="117"/>
       <c r="C26" s="19"/>
       <c r="D26" s="10"/>
       <c r="E26" s="8"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="128"/>
+      <c r="G26" s="114"/>
       <c r="H26" s="8"/>
       <c r="I26" s="11"/>
       <c r="J26" s="8"/>
@@ -2657,12 +2657,12 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="16"/>
-      <c r="B27" s="131"/>
+      <c r="B27" s="117"/>
       <c r="C27" s="19"/>
       <c r="D27" s="10"/>
       <c r="E27" s="8"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="128"/>
+      <c r="G27" s="114"/>
       <c r="H27" s="8"/>
       <c r="I27" s="11"/>
       <c r="J27" s="8"/>
@@ -2690,12 +2690,12 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="16"/>
-      <c r="B28" s="131"/>
+      <c r="B28" s="117"/>
       <c r="C28" s="19"/>
       <c r="D28" s="10"/>
       <c r="E28" s="8"/>
       <c r="F28" s="10"/>
-      <c r="G28" s="128"/>
+      <c r="G28" s="114"/>
       <c r="H28" s="8"/>
       <c r="I28" s="11"/>
       <c r="J28" s="8"/>
@@ -2723,12 +2723,12 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="16"/>
-      <c r="B29" s="131"/>
+      <c r="B29" s="117"/>
       <c r="C29" s="19"/>
       <c r="D29" s="10"/>
       <c r="E29" s="8"/>
       <c r="F29" s="10"/>
-      <c r="G29" s="128"/>
+      <c r="G29" s="114"/>
       <c r="H29" s="8"/>
       <c r="I29" s="11"/>
       <c r="J29" s="8"/>
@@ -2756,12 +2756,12 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="16"/>
-      <c r="B30" s="131"/>
+      <c r="B30" s="117"/>
       <c r="C30" s="19"/>
       <c r="D30" s="10"/>
       <c r="E30" s="8"/>
       <c r="F30" s="10"/>
-      <c r="G30" s="128"/>
+      <c r="G30" s="114"/>
       <c r="H30" s="8"/>
       <c r="I30" s="11"/>
       <c r="J30" s="8"/>
@@ -2789,12 +2789,12 @@
     </row>
     <row r="31" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
-      <c r="B31" s="131"/>
+      <c r="B31" s="117"/>
       <c r="C31" s="19"/>
       <c r="D31" s="10"/>
       <c r="E31" s="8"/>
       <c r="F31" s="10"/>
-      <c r="G31" s="128"/>
+      <c r="G31" s="114"/>
       <c r="H31" s="8"/>
       <c r="I31" s="11"/>
       <c r="J31" s="8"/>
@@ -2856,7 +2856,7 @@
       <c r="D33" s="70"/>
       <c r="E33" s="69"/>
       <c r="F33" s="70"/>
-      <c r="G33" s="129"/>
+      <c r="G33" s="115"/>
       <c r="H33" s="110" t="s">
         <v>88</v>
       </c>
@@ -2889,7 +2889,7 @@
       <c r="D34" s="70"/>
       <c r="E34" s="69"/>
       <c r="F34" s="70"/>
-      <c r="G34" s="129"/>
+      <c r="G34" s="115"/>
       <c r="H34" s="69"/>
       <c r="I34" s="71"/>
       <c r="J34" s="109"/>
@@ -2927,16 +2927,16 @@
       <c r="I35" s="74"/>
       <c r="J35" s="109"/>
       <c r="K35" s="109"/>
-      <c r="L35" s="113" t="s">
+      <c r="L35" s="118" t="s">
         <v>87</v>
       </c>
-      <c r="M35" s="113"/>
-      <c r="N35" s="113"/>
-      <c r="O35" s="113"/>
-      <c r="P35" s="113"/>
-      <c r="Q35" s="113"/>
-      <c r="R35" s="113"/>
-      <c r="S35" s="113"/>
+      <c r="M35" s="118"/>
+      <c r="N35" s="118"/>
+      <c r="O35" s="118"/>
+      <c r="P35" s="118"/>
+      <c r="Q35" s="118"/>
+      <c r="R35" s="118"/>
+      <c r="S35" s="118"/>
       <c r="T35" s="73"/>
       <c r="U35" s="53"/>
       <c r="V35"/>
@@ -3022,8 +3022,8 @@
   </sheetPr>
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -3044,38 +3044,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="str">
+      <c r="A1" s="130" t="str">
         <f>SUBSTITUTE("Finales "&amp;Voorronde!C2,"Rayonkampioenschappen", "RK")</f>
         <v>Finales RK Indoor, seizoen, Rayon#, klasse</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="91"/>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
       <c r="E3" s="91"/>
       <c r="F3" s="91"/>
       <c r="G3" s="91"/>
-      <c r="H3" s="124" t="s">
+      <c r="H3" s="129" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
       <c r="K3" s="91"/>
       <c r="L3" s="91"/>
     </row>
@@ -3377,11 +3377,11 @@
       <c r="E23" s="91"/>
       <c r="F23" s="33"/>
       <c r="G23" s="91"/>
-      <c r="H23" s="126" t="s">
+      <c r="H23" s="131" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="126"/>
-      <c r="J23" s="126"/>
+      <c r="I23" s="131"/>
+      <c r="J23" s="131"/>
       <c r="K23" s="91"/>
       <c r="L23" s="91"/>
     </row>
@@ -3509,11 +3509,11 @@
       <c r="E31" s="91"/>
       <c r="F31" s="33"/>
       <c r="G31" s="91"/>
-      <c r="H31" s="126" t="s">
+      <c r="H31" s="131" t="s">
         <v>29</v>
       </c>
-      <c r="I31" s="126"/>
-      <c r="J31" s="126"/>
+      <c r="I31" s="131"/>
+      <c r="J31" s="131"/>
       <c r="K31" s="92"/>
       <c r="L31" s="91"/>
     </row>
@@ -4056,8 +4056,8 @@
   </sheetPr>
   <dimension ref="A1:X97"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:R1"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4085,27 +4085,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="23" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="str">
+      <c r="A1" s="130" t="str">
         <f>"Finales "&amp;Voorronde!C2</f>
         <v>Finales Rayonkampioenschappen Indoor, seizoen, Rayon#, klasse</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="125"/>
-      <c r="R1" s="125"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130"/>
+      <c r="O1" s="130"/>
+      <c r="P1" s="130"/>
+      <c r="Q1" s="130"/>
+      <c r="R1" s="130"/>
     </row>
     <row r="2" spans="1:18" s="23" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="88"/>
@@ -4129,27 +4129,27 @@
     </row>
     <row r="3" spans="1:18" s="23" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="91"/>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="129" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
       <c r="E3" s="91"/>
       <c r="F3" s="91"/>
       <c r="G3" s="91"/>
-      <c r="H3" s="124" t="s">
+      <c r="H3" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
       <c r="K3" s="91"/>
       <c r="L3" s="91"/>
       <c r="M3" s="91"/>
-      <c r="N3" s="124" t="s">
+      <c r="N3" s="129" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="124"/>
-      <c r="P3" s="124"/>
+      <c r="O3" s="129"/>
+      <c r="P3" s="129"/>
       <c r="Q3" s="91"/>
       <c r="R3" s="91"/>
     </row>
@@ -4599,11 +4599,11 @@
       <c r="K23" s="92"/>
       <c r="L23" s="33"/>
       <c r="M23" s="91"/>
-      <c r="N23" s="126" t="s">
+      <c r="N23" s="131" t="s">
         <v>28</v>
       </c>
-      <c r="O23" s="126"/>
-      <c r="P23" s="126"/>
+      <c r="O23" s="131"/>
+      <c r="P23" s="131"/>
       <c r="Q23" s="91"/>
       <c r="R23" s="91"/>
     </row>
@@ -4787,11 +4787,11 @@
       <c r="K31" s="92"/>
       <c r="L31" s="33"/>
       <c r="M31" s="91"/>
-      <c r="N31" s="126" t="s">
+      <c r="N31" s="131" t="s">
         <v>29</v>
       </c>
-      <c r="O31" s="126"/>
-      <c r="P31" s="126"/>
+      <c r="O31" s="131"/>
+      <c r="P31" s="131"/>
       <c r="Q31" s="92"/>
       <c r="R31" s="91"/>
     </row>
@@ -5615,7 +5615,7 @@
   </sheetPr>
   <dimension ref="A1:X97"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
@@ -5649,33 +5649,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="125" t="str">
+      <c r="A1" s="130" t="str">
         <f>"Finales "&amp;Voorronde!C2</f>
         <v>Finales Rayonkampioenschappen Indoor, seizoen, Rayon#, klasse</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="125"/>
-      <c r="R1" s="125"/>
-      <c r="S1" s="125"/>
-      <c r="T1" s="125"/>
-      <c r="U1" s="125"/>
-      <c r="V1" s="125"/>
-      <c r="W1" s="125"/>
-      <c r="X1" s="125"/>
+      <c r="B1" s="130"/>
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130"/>
+      <c r="O1" s="130"/>
+      <c r="P1" s="130"/>
+      <c r="Q1" s="130"/>
+      <c r="R1" s="130"/>
+      <c r="S1" s="130"/>
+      <c r="T1" s="130"/>
+      <c r="U1" s="130"/>
+      <c r="V1" s="130"/>
+      <c r="W1" s="130"/>
+      <c r="X1" s="130"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="88"/>
@@ -5689,35 +5689,35 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="26"/>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
       <c r="E3" s="93"/>
       <c r="F3" s="91"/>
       <c r="G3" s="91"/>
-      <c r="H3" s="124" t="s">
+      <c r="H3" s="129" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
       <c r="K3" s="91"/>
       <c r="L3" s="91"/>
       <c r="M3" s="91"/>
-      <c r="N3" s="124" t="s">
+      <c r="N3" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="124"/>
-      <c r="P3" s="124"/>
+      <c r="O3" s="129"/>
+      <c r="P3" s="129"/>
       <c r="Q3" s="91"/>
       <c r="R3" s="91"/>
       <c r="S3" s="91"/>
-      <c r="T3" s="124" t="s">
+      <c r="T3" s="129" t="s">
         <v>25</v>
       </c>
-      <c r="U3" s="124"/>
-      <c r="V3" s="124"/>
+      <c r="U3" s="129"/>
+      <c r="V3" s="129"/>
       <c r="W3" s="91"/>
       <c r="X3" s="91"/>
     </row>
@@ -6339,11 +6339,11 @@
       <c r="Q23" s="92"/>
       <c r="R23" s="33"/>
       <c r="S23" s="91"/>
-      <c r="T23" s="126" t="s">
+      <c r="T23" s="131" t="s">
         <v>28</v>
       </c>
-      <c r="U23" s="126"/>
-      <c r="V23" s="126"/>
+      <c r="U23" s="131"/>
+      <c r="V23" s="131"/>
       <c r="W23" s="91"/>
       <c r="X23" s="91"/>
     </row>
@@ -6591,11 +6591,11 @@
       <c r="Q31" s="92"/>
       <c r="R31" s="33"/>
       <c r="S31" s="91"/>
-      <c r="T31" s="126" t="s">
+      <c r="T31" s="131" t="s">
         <v>29</v>
       </c>
-      <c r="U31" s="126"/>
-      <c r="V31" s="126"/>
+      <c r="U31" s="131"/>
+      <c r="V31" s="131"/>
       <c r="W31" s="92"/>
       <c r="X31" s="91"/>
     </row>

</xml_diff>

<commit_message>
Enable merging of small RK classes
</commit_message>
<xml_diff>
--- a/CompLaagRayon/files/template-excel-rk-indoor-indiv.xlsx
+++ b/CompLaagRayon/files/template-excel-rk-indoor-indiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects Ramon\Websites\NHB-applicaties\Excel programma's\RK excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFE3BAD-D6F3-4FB7-9138-AB16D5E7669A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787D6B36-D30B-4F57-811B-48F7974FF740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="2175" windowWidth="18195" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11670" yWindow="570" windowWidth="14880" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uitleg" sheetId="3" r:id="rId1"/>
@@ -406,9 +406,6 @@
     <t>De exacte waardes die je invoert zijn niet van belang, als er maar verschil ontstaat en de velden niet meer geel zijn. Hoger = beter.</t>
   </si>
   <si>
-    <t>Resultaat van de shoot-off / telling moet ingevoerd worden in kolom M. Dit wordt als decimaal toegevoegd aan het resultaat.</t>
-  </si>
-  <si>
     <t>Bij invoeren van een shoot-off resultaat moet de sporter die door mag de hoogste invoer krijgen. Je kan bijvoorbeeld 10 en 9 invoeren. Bij gelijke score met "het dichts bij het midden" kan je een decimaal invoeren, bijvoorbeeld 10,1 en 10,0. Het programma zal een sterretje tonen bij het beste resultaat. Bij opnieuw schieten (beslissing scheidsrechter) hoef je alleen het uiteindelijke resultaat in te voeren.</t>
   </si>
   <si>
@@ -527,6 +524,9 @@
       </rPr>
       <t>: mh-support@handboogsport.nl</t>
     </r>
+  </si>
+  <si>
+    <t>Resultaat van de shoot-off / telling moet ingevoerd worden in kolom R. Dit wordt als decimaal toegevoegd aan het resultaat.</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="76"/>
     </row>
@@ -1485,7 +1485,7 @@
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="76"/>
       <c r="B6" s="77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1583,7 +1583,7 @@
     <row r="24" spans="1:2" ht="45.75" x14ac:dyDescent="0.2">
       <c r="A24" s="76"/>
       <c r="B24" s="77" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1605,7 +1605,7 @@
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="76"/>
       <c r="B28" s="77" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1621,13 +1621,13 @@
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="76"/>
       <c r="B31" s="77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="76"/>
       <c r="B32" s="77" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1649,13 +1649,13 @@
     <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="76"/>
       <c r="B36" s="77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="76"/>
       <c r="B37" s="77" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.2">
@@ -1713,7 +1713,7 @@
     <row r="47" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A47" s="76"/>
       <c r="B47" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1729,7 +1729,7 @@
     <row r="50" spans="1:2" s="49" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A50" s="78"/>
       <c r="B50" s="83" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1757,7 +1757,7 @@
   </sheetPr>
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1816,7 +1816,7 @@
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="122" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" s="123"/>
       <c r="E2" s="123"/>
@@ -1851,7 +1851,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="128" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I3" s="128"/>
       <c r="J3" s="126" t="s">
@@ -1912,11 +1912,11 @@
         <v>2</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="112" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>8</v>
@@ -1939,7 +1939,7 @@
         <v>20</v>
       </c>
       <c r="T5" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U5" s="14" t="s">
         <v>19</v>
@@ -1964,7 +1964,7 @@
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
       <c r="R6" s="84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="S6" s="20" t="s">
         <v>21</v>
@@ -1984,10 +1984,10 @@
         <v>100001</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G7" s="114">
         <v>100</v>
@@ -2840,7 +2840,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B33" s="64"/>
       <c r="C33" s="69"/>
@@ -2849,7 +2849,7 @@
       <c r="F33" s="70"/>
       <c r="G33" s="115"/>
       <c r="H33" s="110" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I33" s="71"/>
       <c r="J33" s="69"/>
@@ -2919,7 +2919,7 @@
       <c r="J35" s="109"/>
       <c r="K35" s="109"/>
       <c r="L35" s="118" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M35" s="118"/>
       <c r="N35" s="118"/>
@@ -2949,7 +2949,7 @@
         <v>2</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H36" s="14"/>
       <c r="I36" s="13" t="s">

</xml_diff>